<commit_message>
Add administrator role request
</commit_message>
<xml_diff>
--- a/Parser/Example/Doc.xlsx
+++ b/Parser/Example/Doc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\PersonalWork\Scripts\ExcelToJsonParser\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE2F70-67B1-4096-809B-DBADE3A0ABD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCC59FC-EF35-4F93-8886-B57FE0FCA5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
   <si>
     <t>season</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>feature_name</t>
+  </si>
+  <si>
+    <t>field11</t>
+  </si>
+  <si>
+    <t>$bool</t>
   </si>
 </sst>
 </file>
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K145"/>
+  <dimension ref="A2:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,39 +662,36 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
+      <c r="C17">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +699,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,59 +710,56 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,18 +767,18 @@
         <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,48 +786,48 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,15 +835,18 @@
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,7 +854,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -856,52 +862,48 @@
         <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
-        <f>CONCATENATE(A$8,"-", B$8)</f>
-        <v>season-field5</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,166 +912,166 @@
         <v>season-field5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>CONCATENATE(A$43,"-", B$43)</f>
-        <v>season-field5-$arr</v>
+        <f>CONCATENATE(A$8,"-", B$8)</f>
+        <v>season-field5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>CONCATENATE(A$43,"-", B$43)</f>
+        <f>CONCATENATE(A$44,"-", B$44)</f>
         <v>season-field5-$arr</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>CONCATENATE(A$43,"-", B$43)</f>
+        <f>CONCATENATE(A$44,"-", B$44)</f>
         <v>season-field5-$arr</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>CONCATENATE(A$44,"-", B$44)</f>
+        <v>season-field5-$arr</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>CONCATENATE(A$44,"-", B$44)</f>
-        <v>season-field5-$arr-0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>CONCATENATE(A$44, "-", B$44)</f>
+        <f>CONCATENATE(A$45,"-", B$45)</f>
         <v>season-field5-$arr-0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>CONCATENATE(A$44,"-", B$44)</f>
+        <f>CONCATENATE(A$45, "-", B$45)</f>
         <v>season-field5-$arr-0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>CONCATENATE(A$49,"-", B$49)</f>
-        <v>season-field5-$arr-0-field5_0_1</v>
+        <f>CONCATENATE(A$45,"-", B$45)</f>
+        <v>season-field5-$arr-0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>CONCATENATE(A$50,"-", B$50)</f>
+        <v>season-field5-$arr-0-field5_0_1</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>CONCATENATE(A$51,"-", B$51)</f>
         <v>season-field5-$arr-0-field5_0_2</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>CONCATENATE(A$45,"-", B$45)</f>
-        <v>season-field5-$arr-1</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>CONCATENATE(A$45,"-", B$45)</f>
+        <f>CONCATENATE(A$46,"-", B$46)</f>
         <v>season-field5-$arr-1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>47</v>
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>CONCATENATE(A$55,"-", B$55)</f>
+        <f>CONCATENATE(A$46,"-", B$46)</f>
+        <v>season-field5-$arr-1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f>CONCATENATE(A$56,"-", B$56)</f>
         <v>season-field5-$arr-1-field5_1_0</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f>CONCATENATE(A$46,"-", B$46)</f>
-        <v>season-field5-$arr-2</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>CONCATENATE(A$58)</f>
+        <f>CONCATENATE(A$47,"-", B$47)</f>
         <v>season-field5-$arr-2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>47</v>
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>CONCATENATE(A$59,"-", B$59)</f>
+        <f>CONCATENATE(A$59)</f>
+        <v>season-field5-$arr-2</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f>CONCATENATE(A$60,"-", B$60)</f>
         <v>season-field5-$arr-2-field5_1_0</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
-        <f>CONCATENATE(A$9, "-", B$9)</f>
-        <v>season-field6</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,19 +1080,19 @@
         <v>season-field6</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f>CONCATENATE(A$9, "-", B$9)</f>
+        <v>season-field6</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
-        <f>CONCATENATE(A$10, "-", B$10)</f>
-        <v>season-field7</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,112 +1101,112 @@
         <v>season-field7</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>CONCATENATE(A$10, "-", B$10)</f>
+        <v>season-field7</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
-        <f>CONCATENATE(A$66, "-", B$66)</f>
-        <v>season-field7-$arr</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>CONCATENATE(A$66, "-", B$66)</f>
+        <f>CONCATENATE(A$67, "-", B$67)</f>
         <v>season-field7-$arr</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>CONCATENATE(A$66, "-", B$66)</f>
+        <f>CONCATENATE(A$67, "-", B$67)</f>
         <v>season-field7-$arr</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="str">
+        <f>CONCATENATE(A$67, "-", B$67)</f>
+        <v>season-field7-$arr</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f>CONCATENATE(A$69, "-", B$69)</f>
-        <v>season-field7-$arr-0</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>CONCATENATE(A$69, "-", B$69)</f>
+        <f>CONCATENATE(A$70, "-", B$70)</f>
         <v>season-field7-$arr-0</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="str">
+        <f>CONCATENATE(A$70, "-", B$70)</f>
+        <v>season-field7-$arr-0</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
-        <f>CONCATENATE(A$70, "-", B$70)</f>
-        <v>season-field7-$arr-1</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f>CONCATENATE(A$70, "-", B$70)</f>
+        <f>CONCATENATE(A$71, "-", B$71)</f>
         <v>season-field7-$arr-1</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="str">
+        <f>CONCATENATE(A$71, "-", B$71)</f>
+        <v>season-field7-$arr-1</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="str">
         <f>CONCATENATE(A$11, "-", B$11)</f>
         <v>season-field8</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="str">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="str">
         <f>CONCATENATE(A$12, "-", B$12)</f>
         <v>season-field9</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
-        <f>CONCATENATE(A$13, "-", B$13)</f>
-        <v>season-field10</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,120 +1215,133 @@
         <v>season-field10</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f>CONCATENATE(A$13, "-", B$13)</f>
+        <v>season-field10</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="str">
-        <f>CONCATENATE(A$83, "-", B$83)</f>
-        <v>season-field10-$arr</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f t="shared" ref="A86:A87" si="0">CONCATENATE(A$83, "-", B$83)</f>
+        <f>CONCATENATE(A$84, "-", B$84)</f>
         <v>season-field10-$arr</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
+        <f t="shared" ref="A87:A88" si="0">CONCATENATE(A$84, "-", B$84)</f>
+        <v>season-field10-$arr</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
         <f t="shared" si="0"/>
         <v>season-field10-$arr</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="str">
-        <f>CONCATENATE(A$85, "-", B$85)</f>
-        <v>season-field10-$arr-1</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f t="shared" ref="A90" si="1">CONCATENATE(A$85, "-", B$85)</f>
+        <f>CONCATENATE(A$86, "-", B$86)</f>
         <v>season-field10-$arr-1</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="str">
+        <f t="shared" ref="A91" si="1">CONCATENATE(A$86, "-", B$86)</f>
+        <v>season-field10-$arr-1</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="str">
-        <f>CONCATENATE(A$90, "-", B$90)</f>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="str">
+        <f>CONCATENATE(A$91, "-", B$91)</f>
         <v>season-field10-$arr-1-field1</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92">
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93">
         <v>12345</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="str">
-        <f>CONCATENATE(A$86, "-", B$86)</f>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="str">
+        <f>CONCATENATE(A$87, "-", B$87)</f>
         <v>season-field10-$arr-2</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="str">
-        <f>CONCATENATE(A$87, "-", B$87)</f>
-        <v>season-field10-$arr-3</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
-        <f>CONCATENATE(A$87, "-", B$87)</f>
+        <f>CONCATENATE(A$88, "-", B$88)</f>
         <v>season-field10-$arr-3</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="str">
+        <f>CONCATENATE(A$88, "-", B$88)</f>
+        <v>season-field10-$arr-3</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="str">
-        <f>CONCATENATE(A$97, "-", B$97)</f>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="str">
+        <f>CONCATENATE(A$98, "-", B$98)</f>
         <v>season-field10-$arr-3-field1</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99">
+      <c r="B100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100">
         <v>12345</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>51</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" t="s">
-        <v>2</v>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="str">
+        <f>CONCATENATE(A$14, "-", B$14)</f>
+        <v>season-field11</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C102" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,7 +1349,10 @@
         <v>51</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1360,7 @@
         <v>51</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1368,7 @@
         <v>51</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,75 +1376,72 @@
         <v>51</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" t="str">
-        <f>CONCATENATE(A109, "-",B109)</f>
-        <v>season1-$type</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C114">
-        <v>123</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
-        <f t="shared" ref="A115:A116" si="2">CONCATENATE(A110, "-",B110)</f>
-        <v>season1-field1</v>
+        <f>CONCATENATE(A110, "-",B110)</f>
+        <v>season1-$type</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C115">
-        <v>0.3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
+        <f t="shared" ref="A116:A117" si="2">CONCATENATE(A111, "-",B111)</f>
+        <v>season1-field1</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" t="str">
         <f t="shared" si="2"/>
         <v>season1-field2</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" t="str">
-        <f>CONCATENATE(A$112, "-",B$112)</f>
-        <v>season1-field3</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>34</v>
+      <c r="C117">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
-        <f>CONCATENATE(A$112, "-",B$112)</f>
+        <f>CONCATENATE(A$113, "-",B$113)</f>
         <v>season1-field3</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" t="str">
+        <f>CONCATENATE(A$113, "-",B$113)</f>
+        <v>season1-field3</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -1434,66 +1449,64 @@
         <v>63</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C124" s="1"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="3"/>
       <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="str">
-        <f>CONCATENATE(A$124,"-",B$124)</f>
-        <v>feature_name-fieldY</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K126" t="s">
-        <v>56</v>
-      </c>
+      <c r="A126" s="3"/>
+      <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="str">
-        <f>CONCATENATE(A$124,"-",B$124)</f>
+        <f>CONCATENATE(A$125,"-",B$125)</f>
         <v>feature_name-fieldY</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C127" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="K127" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="3"/>
+      <c r="A128" s="3" t="str">
+        <f>CONCATENATE(A$125,"-",B$125)</f>
+        <v>feature_name-fieldY</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C128" s="1"/>
+      <c r="K128" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="str">
-        <f>CONCATENATE(A$127,"-",B$127)</f>
-        <v>feature_name-fieldY-$arr</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A129" s="3"/>
       <c r="C129" s="1"/>
-      <c r="K129" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="str">
-        <f>CONCATENATE(A$127,"-",B$127)</f>
+        <f>CONCATENATE(A$128,"-",B$128)</f>
         <v>feature_name-fieldY-$arr</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C130" s="1"/>
       <c r="K130" t="s">
@@ -1501,152 +1514,165 @@
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="3"/>
+      <c r="A131" s="3" t="str">
+        <f>CONCATENATE(A$128,"-",B$128)</f>
+        <v>feature_name-fieldY-$arr</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C131" s="1"/>
+      <c r="K131" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="str">
-        <f>CONCATENATE(A$129,"-",B$129)</f>
-        <v>feature_name-fieldY-$arr-0</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I132" t="s">
-        <v>56</v>
-      </c>
+      <c r="A132" s="3"/>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="str">
-        <f t="shared" ref="A133:A134" si="3">CONCATENATE(A$129,"-",B$129)</f>
+        <f>CONCATENATE(A$130,"-",B$130)</f>
         <v>feature_name-fieldY-$arr-0</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C133" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I133" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="str">
+        <f t="shared" ref="A134:A135" si="3">CONCATENATE(A$130,"-",B$130)</f>
+        <v>feature_name-fieldY-$arr-0</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="str">
         <f t="shared" si="3"/>
         <v>feature_name-fieldY-$arr-0</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C134" s="1"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="3"/>
       <c r="C135" s="1"/>
-      <c r="E135" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="str">
-        <f>CONCATENATE(A$130,"-",B$130)</f>
-        <v>feature_name-fieldY-$arr-1</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I136" t="s">
+      <c r="A136" s="3"/>
+      <c r="C136" s="1"/>
+      <c r="E136" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="str">
-        <f t="shared" ref="A137:A138" si="4">CONCATENATE(A$130,"-",B$130)</f>
+        <f>CONCATENATE(A$131,"-",B$131)</f>
         <v>feature_name-fieldY-$arr-1</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C137" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I137" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="str">
+        <f t="shared" ref="A138:A139" si="4">CONCATENATE(A$131,"-",B$131)</f>
+        <v>feature_name-fieldY-$arr-1</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="str">
         <f t="shared" si="4"/>
         <v>feature_name-fieldY-$arr-1</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C138" s="1"/>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="3"/>
       <c r="C139" s="1"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="str">
-        <f>CONCATENATE(A$133,"-",B$133)</f>
-        <v>feature_name-fieldY-$arr-0-field0</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H140" t="s">
-        <v>56</v>
-      </c>
+      <c r="A140" s="3"/>
+      <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="str">
         <f>CONCATENATE(A$134,"-",B$134)</f>
-        <v>feature_name-fieldY-$arr-0-field1</v>
+        <v>feature_name-fieldY-$arr-0-field0</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H141" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="3"/>
-    </row>
-    <row r="143" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="str">
-        <f>CONCATENATE(A$137,"-",B$137)</f>
-        <v>feature_name-fieldY-$arr-1-field0</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="str">
+        <f>CONCATENATE(A$135,"-",B$135)</f>
+        <v>feature_name-fieldY-$arr-0-field1</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H142" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143" s="3"/>
+    </row>
+    <row r="144" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="str">
         <f>CONCATENATE(A$138,"-",B$138)</f>
+        <v>feature_name-fieldY-$arr-1-field0</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="str">
+        <f>CONCATENATE(A$139,"-",B$139)</f>
         <v>feature_name-fieldY-$arr-1-field1</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144" s="1" t="s">
+      <c r="B145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H144" t="s">
+      <c r="H145" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H145" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add repeatable elements operator
</commit_message>
<xml_diff>
--- a/Parser/Example/Doc.xlsx
+++ b/Parser/Example/Doc.xlsx
@@ -8,13 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0959346-1367-4F84-9575-FADC2E12E8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C9162-94A5-419D-B4B1-568F1867223A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleSheetName" sheetId="1" r:id="rId1"/>
+    <sheet name="RepeatableArray" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">RepeatableArray!$A$19</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="74">
   <si>
     <t>season</t>
   </si>
@@ -223,13 +233,37 @@
   </si>
   <si>
     <t>$bool</t>
+  </si>
+  <si>
+    <t>PlayerLevel</t>
+  </si>
+  <si>
+    <t>$rep_start_row</t>
+  </si>
+  <si>
+    <t>$rep_end_row</t>
+  </si>
+  <si>
+    <t>$rep_values</t>
+  </si>
+  <si>
+    <t>$ref</t>
+  </si>
+  <si>
+    <t>$rep_node</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +277,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -260,16 +301,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,4 +1743,438 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D932CE5A-FC33-48B4-9C1F-56F9576B1702}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:L78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="7" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>CONCATENATE(A13,"-",B13)</f>
+        <v>root-$arr</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>CONCATENATE(A14,"-",B14)</f>
+        <v>root-$arr-1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>CONCATENATE(A14,"-",B14)</f>
+        <v>root-$arr-1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>CONCATENATE(A16,"-",B16)</f>
+        <v>root-$arr-1-field1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>CONCATENATE(A13,"-",B13)</f>
+        <v>root-$arr</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>CONCATENATE(A18,"-",B18)</f>
+        <v>root-$arr-2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>CONCATENATE(A19,"-",B19)</f>
+        <v>root-$arr-2-$rep_node</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20">
+        <f>ROW(H3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>CONCATENATE(A19,"-",B19)</f>
+        <v>root-$arr-2-$rep_node</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <f>ROW(H7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>CONCATENATE(A19,"-",B19)</f>
+        <v>root-$arr-2-$rep_node</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>CONCATENATE(A22,"-",B22)</f>
+        <v>root-$arr-2-$rep_node-$rep_values</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>CONCATENATE(A22,"-",B22)</f>
+        <v>root-$arr-2-$rep_node-$rep_values</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" outlineLevel="6" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CONCATENATE(A24,"-",B24)</f>
+        <v>root-$arr-2-$rep_node-$rep_values-field1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>CONCATENATE(A22,"-",B22)</f>
+        <v>root-$arr-2-$rep_node-$rep_values</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" outlineLevel="6" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>CONCATENATE(A26,"-",B26)</f>
+        <v>root-$arr-2-$rep_node-$rep_values-field2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" outlineLevel="7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>CONCATENATE(A27,"-",B27)</f>
+        <v>root-$arr-2-$rep_node-$rep_values-field2-$ref</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <f>COLUMN(H2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" outlineLevel="3" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>CONCATENATE(A13,"-",B13)</f>
+        <v>root-$arr</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>CONCATENATE(A30,"-",B30)</f>
+        <v>root-$arr-3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>CONCATENATE(A31,"-",B31)</f>
+        <v>root-$arr-3-$rep_node</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32">
+        <f>ROW(H3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>CONCATENATE(A31,"-",B31)</f>
+        <v>root-$arr-3-$rep_node</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33">
+        <f>ROW(H7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>CONCATENATE(A31,"-",B31)</f>
+        <v>root-$arr-3-$rep_node</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>CONCATENATE(A34,"-",B34)</f>
+        <v>root-$arr-3-$rep_node-$rep_values</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>CONCATENATE(A34,"-",B34)</f>
+        <v>root-$arr-3-$rep_node-$rep_values</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" outlineLevel="6" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>CONCATENATE(A36,"-",B36)</f>
+        <v>root-$arr-3-$rep_node-$rep_values-field1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>CONCATENATE(A34,"-",B34)</f>
+        <v>root-$arr-3-$rep_node-$rep_values</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" outlineLevel="6" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>CONCATENATE(A38,"-",B38)</f>
+        <v>root-$arr-3-$rep_node-$rep_values-field2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" outlineLevel="7" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>CONCATENATE(A39,"-",B39)</f>
+        <v>root-$arr-3-$rep_node-$rep_values-field2-$ref</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <f>COLUMN(H2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" outlineLevel="5" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>